<commit_message>
normalised job ads analysis
</commit_message>
<xml_diff>
--- a/Job_Data/Computer Science Domain New Data/431/merged_domain_analysis.xlsx
+++ b/Job_Data/Computer Science Domain New Data/431/merged_domain_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishwas\Desktop\Thesis\ontology_translation\Job_Data\Computer Science Domain New Data\431\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC561250-6DFC-4174-A6FD-522BD3A380D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BB3F3A-0B64-4DA4-B7A9-04F38F3B3359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -7694,7 +7694,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{87E6A63E-4C1B-4F7E-BCAD-86DE325D265A}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{87E6A63E-4C1B-4F7E-BCAD-86DE325D265A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A2:J179" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
@@ -8746,7 +8746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -23791,7 +23791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9970F996-DE8C-43B4-8B68-4118888A29C7}">
   <dimension ref="A2:J179"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add top and first domain analysis data
</commit_message>
<xml_diff>
--- a/Job_Data/Computer Science Domain New Data/431/merged_domain_analysis.xlsx
+++ b/Job_Data/Computer Science Domain New Data/431/merged_domain_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishwas\Desktop\Thesis\ontology_translation\Job_Data\Computer Science Domain New Data\431\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BB3F3A-0B64-4DA4-B7A9-04F38F3B3359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC266B9F-431E-4917-BCF2-8C4823180983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -7694,7 +7694,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{87E6A63E-4C1B-4F7E-BCAD-86DE325D265A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{87E6A63E-4C1B-4F7E-BCAD-86DE325D265A}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A2:J179" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
@@ -8746,8 +8746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1366"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23791,7 +23791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9970F996-DE8C-43B4-8B68-4118888A29C7}">
   <dimension ref="A2:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>